<commit_message>
FIX: New generated dynamic_range.xlsx in windows without hardcoded error strings
</commit_message>
<xml_diff>
--- a/tests/resources/DYNAMIC_RANGE.xlsx
+++ b/tests/resources/DYNAMIC_RANGE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace_local\xlcalculator\tests\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D2A153B4-6912-46AF-A2DB-19F2D5040C85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8416B77C-2768-495B-BBEA-8121820C3634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6144" yWindow="6144" windowWidth="34560" windowHeight="18600" xr2:uid="{2712C351-5446-4FC3-85C3-2AC205215D06}"/>
+    <workbookView xWindow="6144" yWindow="6144" windowWidth="34560" windowHeight="18600" xr2:uid="{5CAE1DF7-95EE-40DB-B171-075F5E8EFCA9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -460,7 +460,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B02B36FF-3D5A-4ACD-BD78-64125DC36851}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{402B1F50-AEC2-40F9-AEDD-C9B414C48F95}">
   <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -666,33 +666,33 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="I9" t="str">
-        <f ca="1">IF(ISERROR(OFFSET(A1, -1, 0)), "#VALUE!", OFFSET(A1, -1, 0))</f>
-        <v>#VALUE!</v>
+      <c r="I9" t="e">
+        <f ca="1">OFFSET(A1, -1, 0)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="G10" t="str">
-        <f>IF(ISERROR(INDEX(A1:E5, 6, 1)), "#REF!", INDEX(A1:E5, 6, 1))</f>
+      <c r="G10" t="e">
+        <f>INDEX(A1:E5, 6, 1)</f>
         <v>#REF!</v>
       </c>
-      <c r="I10" t="str">
-        <f ca="1">IF(ISERROR(OFFSET(A1, 0, -1)), "#VALUE!", OFFSET(A1, 0, -1))</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M10" t="str">
-        <f ca="1">IF(ISERROR(INDIRECT(K5)), "#NAME?", INDIRECT(K5))</f>
-        <v>#NAME?</v>
+      <c r="I10" t="e">
+        <f ca="1">OFFSET(A1, 0, -1)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="M10" t="e">
+        <f ca="1">INDIRECT(K5)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="G11" t="str">
-        <f>IF(ISERROR(INDEX(A1:E5, 1, 6)), "#REF!", INDEX(A1:E5, 1, 6))</f>
+      <c r="G11" t="e">
+        <f>INDEX(A1:E5, 1, 6)</f>
         <v>#REF!</v>
       </c>
-      <c r="M11" t="str">
-        <f ca="1">IF(ISERROR(INDIRECT("")), "#NAME?", INDIRECT(""))</f>
-        <v>#NAME?</v>
+      <c r="M11" t="e">
+        <f ca="1">INDIRECT("")</f>
+        <v>#REF!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>